<commit_message>
v: fixed SVOD_DATA, reconfigure comparison. Fix additional functions
</commit_message>
<xml_diff>
--- a/real/140 РАСПОРЯЖЕНИЕ ЗА 12МЕСЯЦЕВ 2015.xlsx
+++ b/real/140 РАСПОРЯЖЕНИЕ ЗА 12МЕСЯЦЕВ 2015.xlsx
@@ -196,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -222,6 +222,7 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -529,7 +530,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,6 +538,9 @@
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="145.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -614,7 +618,7 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="9">
         <v>42223.423611111109</v>
       </c>
       <c r="F2" t="s">
@@ -641,7 +645,7 @@
       <c r="M2">
         <v>50067818</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="9">
         <v>42237.708333333336</v>
       </c>
       <c r="O2">
@@ -676,7 +680,7 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="9">
         <v>42223.423611111109</v>
       </c>
       <c r="F3" t="s">
@@ -703,7 +707,7 @@
       <c r="M3">
         <v>50067818</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="9">
         <v>42237.708333333336</v>
       </c>
       <c r="O3">
@@ -738,7 +742,7 @@
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="9">
         <v>42223.423611111109</v>
       </c>
       <c r="F4" t="s">
@@ -765,7 +769,7 @@
       <c r="M4">
         <v>50067818</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="9">
         <v>42237.708333333336</v>
       </c>
       <c r="O4">
@@ -800,7 +804,7 @@
       <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="9">
         <v>42223.423611111109</v>
       </c>
       <c r="F5" t="s">
@@ -827,7 +831,7 @@
       <c r="M5">
         <v>50067818</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="9">
         <v>42237.708333333336</v>
       </c>
       <c r="O5">
@@ -862,7 +866,7 @@
       <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="9">
         <v>42223.423611111109</v>
       </c>
       <c r="F6" t="s">
@@ -883,7 +887,7 @@
       <c r="M6">
         <v>50067818</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="9">
         <v>42237.708333333336</v>
       </c>
       <c r="O6">
@@ -912,7 +916,7 @@
       <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="9">
         <v>42223.423611111109</v>
       </c>
       <c r="F7" t="s">
@@ -933,7 +937,7 @@
       <c r="M7">
         <v>50067818</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="9">
         <v>42237.708333333336</v>
       </c>
       <c r="O7">
@@ -962,7 +966,7 @@
       <c r="D8" t="s">
         <v>2</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="9">
         <v>42223.423611111109</v>
       </c>
       <c r="F8" t="s">
@@ -983,7 +987,7 @@
       <c r="M8">
         <v>50067818</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="9">
         <v>42237.708333333336</v>
       </c>
       <c r="O8">
@@ -1012,7 +1016,7 @@
       <c r="D9" t="s">
         <v>2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="9">
         <v>42223.423611111109</v>
       </c>
       <c r="F9" t="s">
@@ -1033,7 +1037,7 @@
       <c r="M9">
         <v>50067818</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="9">
         <v>42237.708333333336</v>
       </c>
       <c r="O9">

</xml_diff>